<commit_message>
Committing test class code for SAL-137
</commit_message>
<xml_diff>
--- a/data/sfGroupsData.xlsx
+++ b/data/sfGroupsData.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10416"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10416" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Edit" sheetId="3" r:id="rId1"/>
+    <sheet name="Create" sheetId="1" r:id="rId2"/>
+    <sheet name="Delete" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>strGroupName</t>
   </si>
@@ -35,13 +37,31 @@
     <t>C:\Users\amhas\Pictures\sample images\sample1.jpg</t>
   </si>
   <si>
-    <t>Haseena14</t>
-  </si>
-  <si>
-    <t>Haseena15</t>
-  </si>
-  <si>
-    <t>Haseena16</t>
+    <t>Haseena20</t>
+  </si>
+  <si>
+    <t>Haseena21</t>
+  </si>
+  <si>
+    <t>strGroupDescription</t>
+  </si>
+  <si>
+    <t>TestLeaf</t>
+  </si>
+  <si>
+    <t>strFontName</t>
+  </si>
+  <si>
+    <t>strFontSize</t>
+  </si>
+  <si>
+    <t>Verdana</t>
+  </si>
+  <si>
+    <t>Haseena22</t>
+  </si>
+  <si>
+    <t>Haseena23</t>
   </si>
 </sst>
 </file>
@@ -366,10 +386,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.68359375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -403,10 +470,46 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>